<commit_message>
more improvements to data files and validatoin
</commit_message>
<xml_diff>
--- a/mppsteel/data/import_data/Energy Prices - Static.xlsx
+++ b/mppsteel/data/import_data/Energy Prices - Static.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://systemiq.sharepoint.com/Projects/MPP0006/Shared Documents/6_ Working documents/03 Steel python model/Data Sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{FBE8CABE-D20B-4584-B4F2-78759DF641A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2377E7CB-FC2F-42CB-AB03-8AF1F80514BE}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{FBE8CABE-D20B-4584-B4F2-78759DF641A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E655B00-F916-43D8-B12E-C3EA75949526}"/>
   <bookViews>
-    <workbookView xWindow="1047" yWindow="1047" windowWidth="19200" windowHeight="9613" xr2:uid="{3C9558B5-A0F5-403C-8FC2-4F440354339E}"/>
+    <workbookView xWindow="17320" yWindow="-15410" windowWidth="12310" windowHeight="12870" xr2:uid="{3C9558B5-A0F5-403C-8FC2-4F440354339E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="26">
   <si>
     <t>Year</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Excel Tab</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
@@ -112,9 +109,6 @@
   </si>
   <si>
     <t>Carbon price</t>
-  </si>
-  <si>
-    <t>Price &amp; Emission Parameters</t>
   </si>
   <si>
     <t>Energy Prices - Static</t>
@@ -504,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C37EDE78-E1C1-429F-B011-5D0090943F4A}">
-  <dimension ref="A1:F85"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -515,11 +509,10 @@
     <col min="1" max="1" width="9.29296875" customWidth="1"/>
     <col min="2" max="3" width="18.3515625" customWidth="1"/>
     <col min="4" max="4" width="22.5859375" customWidth="1"/>
-    <col min="5" max="5" width="24.703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.64453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.64453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -530,1741 +523,1486 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>2020</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>2020</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="E3" s="2">
         <f>140*0.877</f>
         <v>122.78</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>2020</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="2">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2">
         <f>75/22*0.877</f>
         <v>2.9897727272727272</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>2020</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>2020</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+        <v>11</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>2020</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>2020</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
         <v>15</v>
       </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="2">
+      <c r="E8" s="2">
         <f>3*0.877</f>
         <v>2.6310000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>2020</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
         <v>17</v>
       </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="2">
+      <c r="E9" s="2">
         <f>12*0.877</f>
         <v>10.524000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>2020</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
         <v>19</v>
       </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="2">
+      <c r="E10" s="2">
         <f>280/28.4*0.877</f>
         <v>8.6464788732394382</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>2020</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
         <v>21</v>
       </c>
-      <c r="D11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="2">
-        <f>F9*2</f>
+      <c r="E11" s="2">
+        <f>E9*2</f>
         <v>21.048000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>2020</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
         <v>23</v>
       </c>
-      <c r="D12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="2">
-        <f>F4</f>
+      <c r="E12" s="2">
+        <f>E4</f>
         <v>2.9897727272727272</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>2020</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
+        <v>24</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>2021</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
         <v>6</v>
       </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>2021</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" s="2">
-        <f t="shared" ref="F15:F75" si="0">140*0.877</f>
+      <c r="E15" s="2">
+        <f t="shared" ref="E15:E75" si="0">140*0.877</f>
         <v>122.78</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>2021</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" s="2">
-        <f t="shared" ref="F16:F76" si="1">75/22*0.877</f>
+        <v>8</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" ref="E16:E76" si="1">75/22*0.877</f>
         <v>2.9897727272727272</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A17">
         <v>2021</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
         <v>11</v>
       </c>
-      <c r="D17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A18">
         <v>2021</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" t="s">
-        <v>26</v>
-      </c>
-      <c r="F18" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
+        <v>11</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A19">
         <v>2021</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" t="s">
-        <v>26</v>
-      </c>
-      <c r="F19" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
+        <v>11</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A20">
         <v>2021</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
         <v>15</v>
       </c>
-      <c r="D20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" t="s">
-        <v>26</v>
-      </c>
-      <c r="F20" s="2">
-        <f t="shared" ref="F20:F80" si="2">3*0.877</f>
+      <c r="E20" s="2">
+        <f t="shared" ref="E20:E80" si="2">3*0.877</f>
         <v>2.6310000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A21">
         <v>2021</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" t="s">
         <v>17</v>
       </c>
-      <c r="D21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" s="2">
-        <f t="shared" ref="F21:F81" si="3">12*0.877</f>
+      <c r="E21" s="2">
+        <f t="shared" ref="E21:E81" si="3">12*0.877</f>
         <v>10.524000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A22">
         <v>2021</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" t="s">
         <v>19</v>
       </c>
-      <c r="D22" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" s="2">
-        <f t="shared" ref="F22:F82" si="4">280/28.4*0.877</f>
+      <c r="E22" s="2">
+        <f t="shared" ref="E22:E82" si="4">280/28.4*0.877</f>
         <v>8.6464788732394382</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A23">
         <v>2021</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" t="s">
         <v>21</v>
       </c>
-      <c r="D23" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" t="s">
-        <v>26</v>
-      </c>
-      <c r="F23" s="2">
-        <f>F21*2</f>
+      <c r="E23" s="2">
+        <f>E21*2</f>
         <v>21.048000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A24">
         <v>2021</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
         <v>23</v>
       </c>
-      <c r="D24" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" s="2">
-        <f>F16</f>
+      <c r="E24" s="2">
+        <f>E16</f>
         <v>2.9897727272727272</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A25">
         <v>2021</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>25</v>
-      </c>
-      <c r="E25" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.5">
+        <v>24</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A26">
         <v>2022</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" t="s">
         <v>6</v>
       </c>
-      <c r="D26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" t="s">
-        <v>26</v>
-      </c>
-      <c r="F26" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A27">
         <v>2022</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" t="s">
-        <v>26</v>
-      </c>
-      <c r="F27" s="2">
+      <c r="E27" s="2">
         <f t="shared" si="0"/>
         <v>122.78</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A28">
         <v>2022</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" t="s">
-        <v>26</v>
-      </c>
-      <c r="F28" s="2">
+        <v>8</v>
+      </c>
+      <c r="E28" s="2">
         <f t="shared" si="1"/>
         <v>2.9897727272727272</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A29">
         <v>2022</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" t="s">
         <v>11</v>
       </c>
-      <c r="D29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" t="s">
-        <v>26</v>
-      </c>
-      <c r="F29" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="E29" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A30">
         <v>2022</v>
       </c>
       <c r="B30" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" t="s">
-        <v>26</v>
-      </c>
-      <c r="F30" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.5">
+        <v>11</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A31">
         <v>2022</v>
       </c>
       <c r="B31" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" t="s">
-        <v>26</v>
-      </c>
-      <c r="F31" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.5">
+        <v>11</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A32">
         <v>2022</v>
       </c>
       <c r="B32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" t="s">
         <v>15</v>
       </c>
-      <c r="D32" t="s">
-        <v>16</v>
-      </c>
-      <c r="E32" t="s">
-        <v>26</v>
-      </c>
-      <c r="F32" s="2">
+      <c r="E32" s="2">
         <f t="shared" si="2"/>
         <v>2.6310000000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A33">
         <v>2022</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" t="s">
         <v>17</v>
       </c>
-      <c r="D33" t="s">
-        <v>18</v>
-      </c>
-      <c r="E33" t="s">
-        <v>26</v>
-      </c>
-      <c r="F33" s="2">
+      <c r="E33" s="2">
         <f t="shared" si="3"/>
         <v>10.524000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A34">
         <v>2022</v>
       </c>
       <c r="B34" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" t="s">
         <v>19</v>
       </c>
-      <c r="D34" t="s">
-        <v>20</v>
-      </c>
-      <c r="E34" t="s">
-        <v>26</v>
-      </c>
-      <c r="F34" s="2">
+      <c r="E34" s="2">
         <f t="shared" si="4"/>
         <v>8.6464788732394382</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A35">
         <v>2022</v>
       </c>
       <c r="B35" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" t="s">
         <v>21</v>
       </c>
-      <c r="D35" t="s">
-        <v>22</v>
-      </c>
-      <c r="E35" t="s">
-        <v>26</v>
-      </c>
-      <c r="F35" s="2">
-        <f>F33*2</f>
+      <c r="E35" s="2">
+        <f>E33*2</f>
         <v>21.048000000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A36">
         <v>2022</v>
       </c>
       <c r="B36" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" t="s">
         <v>23</v>
       </c>
-      <c r="D36" t="s">
-        <v>24</v>
-      </c>
-      <c r="E36" t="s">
-        <v>26</v>
-      </c>
-      <c r="F36" s="2">
-        <f>F28</f>
+      <c r="E36" s="2">
+        <f>E28</f>
         <v>2.9897727272727272</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A37">
         <v>2022</v>
       </c>
       <c r="B37" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D37" t="s">
-        <v>25</v>
-      </c>
-      <c r="E37" t="s">
-        <v>26</v>
-      </c>
-      <c r="F37" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.5">
+        <v>24</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A38">
         <v>2023</v>
       </c>
       <c r="B38" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
         <v>6</v>
       </c>
-      <c r="D38" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38" t="s">
-        <v>26</v>
-      </c>
-      <c r="F38" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="E38" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A39">
         <v>2023</v>
       </c>
       <c r="B39" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" t="s">
-        <v>26</v>
-      </c>
-      <c r="F39" s="2">
+      <c r="E39" s="2">
         <f t="shared" si="0"/>
         <v>122.78</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A40">
         <v>2023</v>
       </c>
       <c r="B40" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" t="s">
-        <v>26</v>
-      </c>
-      <c r="F40" s="2">
+        <v>8</v>
+      </c>
+      <c r="E40" s="2">
         <f t="shared" si="1"/>
         <v>2.9897727272727272</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A41">
         <v>2023</v>
       </c>
       <c r="B41" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
         <v>11</v>
       </c>
-      <c r="D41" t="s">
-        <v>12</v>
-      </c>
-      <c r="E41" t="s">
-        <v>26</v>
-      </c>
-      <c r="F41" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="E41" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A42">
         <v>2023</v>
       </c>
       <c r="B42" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C42" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D42" t="s">
-        <v>12</v>
-      </c>
-      <c r="E42" t="s">
-        <v>26</v>
-      </c>
-      <c r="F42" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.5">
+        <v>11</v>
+      </c>
+      <c r="E42" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A43">
         <v>2023</v>
       </c>
       <c r="B43" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D43" t="s">
-        <v>12</v>
-      </c>
-      <c r="E43" t="s">
-        <v>26</v>
-      </c>
-      <c r="F43" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.5">
+        <v>11</v>
+      </c>
+      <c r="E43" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A44">
         <v>2023</v>
       </c>
       <c r="B44" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C44" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" t="s">
         <v>15</v>
       </c>
-      <c r="D44" t="s">
-        <v>16</v>
-      </c>
-      <c r="E44" t="s">
-        <v>26</v>
-      </c>
-      <c r="F44" s="2">
+      <c r="E44" s="2">
         <f t="shared" si="2"/>
         <v>2.6310000000000002</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A45">
         <v>2023</v>
       </c>
       <c r="B45" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C45" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" t="s">
         <v>17</v>
       </c>
-      <c r="D45" t="s">
-        <v>18</v>
-      </c>
-      <c r="E45" t="s">
-        <v>26</v>
-      </c>
-      <c r="F45" s="2">
+      <c r="E45" s="2">
         <f t="shared" si="3"/>
         <v>10.524000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A46">
         <v>2023</v>
       </c>
       <c r="B46" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" t="s">
         <v>19</v>
       </c>
-      <c r="D46" t="s">
-        <v>20</v>
-      </c>
-      <c r="E46" t="s">
-        <v>26</v>
-      </c>
-      <c r="F46" s="2">
+      <c r="E46" s="2">
         <f t="shared" si="4"/>
         <v>8.6464788732394382</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A47">
         <v>2023</v>
       </c>
       <c r="B47" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C47" t="s">
+        <v>20</v>
+      </c>
+      <c r="D47" t="s">
         <v>21</v>
       </c>
-      <c r="D47" t="s">
-        <v>22</v>
-      </c>
-      <c r="E47" t="s">
-        <v>26</v>
-      </c>
-      <c r="F47" s="2">
-        <f>F45*2</f>
+      <c r="E47" s="2">
+        <f>E45*2</f>
         <v>21.048000000000002</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A48">
         <v>2023</v>
       </c>
       <c r="B48" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C48" t="s">
+        <v>22</v>
+      </c>
+      <c r="D48" t="s">
         <v>23</v>
       </c>
-      <c r="D48" t="s">
-        <v>24</v>
-      </c>
-      <c r="E48" t="s">
-        <v>26</v>
-      </c>
-      <c r="F48" s="2">
-        <f>F40</f>
+      <c r="E48" s="2">
+        <f>E40</f>
         <v>2.9897727272727272</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A49">
         <v>2023</v>
       </c>
       <c r="B49" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C49" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D49" t="s">
-        <v>25</v>
-      </c>
-      <c r="E49" t="s">
-        <v>26</v>
-      </c>
-      <c r="F49" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.5">
+        <v>24</v>
+      </c>
+      <c r="E49" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A50">
         <v>2024</v>
       </c>
       <c r="B50" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C50" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" t="s">
         <v>6</v>
       </c>
-      <c r="D50" t="s">
-        <v>7</v>
-      </c>
-      <c r="E50" t="s">
-        <v>26</v>
-      </c>
-      <c r="F50" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="E50" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A51">
         <v>2024</v>
       </c>
       <c r="B51" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C51" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" t="s">
-        <v>26</v>
-      </c>
-      <c r="F51" s="2">
+      <c r="E51" s="2">
         <f t="shared" si="0"/>
         <v>122.78</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A52">
         <v>2024</v>
       </c>
       <c r="B52" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" t="s">
-        <v>26</v>
-      </c>
-      <c r="F52" s="2">
+        <v>8</v>
+      </c>
+      <c r="E52" s="2">
         <f t="shared" si="1"/>
         <v>2.9897727272727272</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A53">
         <v>2024</v>
       </c>
       <c r="B53" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C53" t="s">
+        <v>10</v>
+      </c>
+      <c r="D53" t="s">
         <v>11</v>
       </c>
-      <c r="D53" t="s">
-        <v>12</v>
-      </c>
-      <c r="E53" t="s">
-        <v>26</v>
-      </c>
-      <c r="F53" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="E53" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A54">
         <v>2024</v>
       </c>
       <c r="B54" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C54" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D54" t="s">
-        <v>12</v>
-      </c>
-      <c r="E54" t="s">
-        <v>26</v>
-      </c>
-      <c r="F54" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.5">
+        <v>11</v>
+      </c>
+      <c r="E54" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A55">
         <v>2024</v>
       </c>
       <c r="B55" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C55" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D55" t="s">
-        <v>12</v>
-      </c>
-      <c r="E55" t="s">
-        <v>26</v>
-      </c>
-      <c r="F55" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.5">
+        <v>11</v>
+      </c>
+      <c r="E55" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A56">
         <v>2024</v>
       </c>
       <c r="B56" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C56" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" t="s">
         <v>15</v>
       </c>
-      <c r="D56" t="s">
-        <v>16</v>
-      </c>
-      <c r="E56" t="s">
-        <v>26</v>
-      </c>
-      <c r="F56" s="2">
+      <c r="E56" s="2">
         <f t="shared" si="2"/>
         <v>2.6310000000000002</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A57">
         <v>2024</v>
       </c>
       <c r="B57" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C57" t="s">
+        <v>16</v>
+      </c>
+      <c r="D57" t="s">
         <v>17</v>
       </c>
-      <c r="D57" t="s">
-        <v>18</v>
-      </c>
-      <c r="E57" t="s">
-        <v>26</v>
-      </c>
-      <c r="F57" s="2">
+      <c r="E57" s="2">
         <f t="shared" si="3"/>
         <v>10.524000000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A58">
         <v>2024</v>
       </c>
       <c r="B58" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C58" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58" t="s">
         <v>19</v>
       </c>
-      <c r="D58" t="s">
-        <v>20</v>
-      </c>
-      <c r="E58" t="s">
-        <v>26</v>
-      </c>
-      <c r="F58" s="2">
+      <c r="E58" s="2">
         <f t="shared" si="4"/>
         <v>8.6464788732394382</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A59">
         <v>2024</v>
       </c>
       <c r="B59" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C59" t="s">
+        <v>20</v>
+      </c>
+      <c r="D59" t="s">
         <v>21</v>
       </c>
-      <c r="D59" t="s">
-        <v>22</v>
-      </c>
-      <c r="E59" t="s">
-        <v>26</v>
-      </c>
-      <c r="F59" s="2">
-        <f>F57*2</f>
+      <c r="E59" s="2">
+        <f>E57*2</f>
         <v>21.048000000000002</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A60">
         <v>2024</v>
       </c>
       <c r="B60" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C60" t="s">
+        <v>22</v>
+      </c>
+      <c r="D60" t="s">
         <v>23</v>
       </c>
-      <c r="D60" t="s">
-        <v>24</v>
-      </c>
-      <c r="E60" t="s">
-        <v>26</v>
-      </c>
-      <c r="F60" s="2">
-        <f>F52</f>
+      <c r="E60" s="2">
+        <f>E52</f>
         <v>2.9897727272727272</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A61">
         <v>2024</v>
       </c>
       <c r="B61" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C61" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D61" t="s">
-        <v>25</v>
-      </c>
-      <c r="E61" t="s">
-        <v>26</v>
-      </c>
-      <c r="F61" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.5">
+        <v>24</v>
+      </c>
+      <c r="E61" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A62">
         <v>2025</v>
       </c>
       <c r="B62" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C62" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" t="s">
         <v>6</v>
       </c>
-      <c r="D62" t="s">
-        <v>7</v>
-      </c>
-      <c r="E62" t="s">
-        <v>26</v>
-      </c>
-      <c r="F62" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="E62" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A63">
         <v>2025</v>
       </c>
       <c r="B63" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C63" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D63" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E63" t="s">
-        <v>26</v>
-      </c>
-      <c r="F63" s="2">
+      <c r="E63" s="2">
         <f t="shared" si="0"/>
         <v>122.78</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A64">
         <v>2025</v>
       </c>
       <c r="B64" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C64" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E64" t="s">
-        <v>26</v>
-      </c>
-      <c r="F64" s="2">
+        <v>8</v>
+      </c>
+      <c r="E64" s="2">
         <f t="shared" si="1"/>
         <v>2.9897727272727272</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A65">
         <v>2025</v>
       </c>
       <c r="B65" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C65" t="s">
+        <v>10</v>
+      </c>
+      <c r="D65" t="s">
         <v>11</v>
       </c>
-      <c r="D65" t="s">
-        <v>12</v>
-      </c>
-      <c r="E65" t="s">
-        <v>26</v>
-      </c>
-      <c r="F65" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="E65" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A66">
         <v>2025</v>
       </c>
       <c r="B66" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C66" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D66" t="s">
-        <v>12</v>
-      </c>
-      <c r="E66" t="s">
-        <v>26</v>
-      </c>
-      <c r="F66" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.5">
+        <v>11</v>
+      </c>
+      <c r="E66" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A67">
         <v>2025</v>
       </c>
       <c r="B67" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C67" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D67" t="s">
-        <v>12</v>
-      </c>
-      <c r="E67" t="s">
-        <v>26</v>
-      </c>
-      <c r="F67" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.5">
+        <v>11</v>
+      </c>
+      <c r="E67" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A68">
         <v>2025</v>
       </c>
       <c r="B68" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C68" t="s">
+        <v>14</v>
+      </c>
+      <c r="D68" t="s">
         <v>15</v>
       </c>
-      <c r="D68" t="s">
-        <v>16</v>
-      </c>
-      <c r="E68" t="s">
-        <v>26</v>
-      </c>
-      <c r="F68" s="2">
+      <c r="E68" s="2">
         <f t="shared" si="2"/>
         <v>2.6310000000000002</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A69">
         <v>2025</v>
       </c>
       <c r="B69" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C69" t="s">
+        <v>16</v>
+      </c>
+      <c r="D69" t="s">
         <v>17</v>
       </c>
-      <c r="D69" t="s">
-        <v>18</v>
-      </c>
-      <c r="E69" t="s">
-        <v>26</v>
-      </c>
-      <c r="F69" s="2">
+      <c r="E69" s="2">
         <f t="shared" si="3"/>
         <v>10.524000000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A70">
         <v>2025</v>
       </c>
       <c r="B70" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C70" t="s">
+        <v>18</v>
+      </c>
+      <c r="D70" t="s">
         <v>19</v>
       </c>
-      <c r="D70" t="s">
-        <v>20</v>
-      </c>
-      <c r="E70" t="s">
-        <v>26</v>
-      </c>
-      <c r="F70" s="2">
+      <c r="E70" s="2">
         <f t="shared" si="4"/>
         <v>8.6464788732394382</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A71">
         <v>2025</v>
       </c>
       <c r="B71" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C71" t="s">
+        <v>20</v>
+      </c>
+      <c r="D71" t="s">
         <v>21</v>
       </c>
-      <c r="D71" t="s">
-        <v>22</v>
-      </c>
-      <c r="E71" t="s">
-        <v>26</v>
-      </c>
-      <c r="F71" s="2">
-        <f>F69*2</f>
+      <c r="E71" s="2">
+        <f>E69*2</f>
         <v>21.048000000000002</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A72">
         <v>2025</v>
       </c>
       <c r="B72" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C72" t="s">
+        <v>22</v>
+      </c>
+      <c r="D72" t="s">
         <v>23</v>
       </c>
-      <c r="D72" t="s">
-        <v>24</v>
-      </c>
-      <c r="E72" t="s">
-        <v>26</v>
-      </c>
-      <c r="F72" s="2">
-        <f>F64</f>
+      <c r="E72" s="2">
+        <f>E64</f>
         <v>2.9897727272727272</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A73">
         <v>2025</v>
       </c>
       <c r="B73" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C73" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D73" t="s">
-        <v>25</v>
-      </c>
-      <c r="E73" t="s">
-        <v>26</v>
-      </c>
-      <c r="F73" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.5">
+        <v>24</v>
+      </c>
+      <c r="E73" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A74">
         <v>2026</v>
       </c>
       <c r="B74" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C74" t="s">
+        <v>5</v>
+      </c>
+      <c r="D74" t="s">
         <v>6</v>
       </c>
-      <c r="D74" t="s">
-        <v>7</v>
-      </c>
-      <c r="E74" t="s">
-        <v>26</v>
-      </c>
-      <c r="F74" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="E74" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A75">
         <v>2026</v>
       </c>
       <c r="B75" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C75" t="s">
+        <v>7</v>
+      </c>
+      <c r="D75" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D75" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E75" t="s">
-        <v>26</v>
-      </c>
-      <c r="F75" s="2">
+      <c r="E75" s="2">
         <f t="shared" si="0"/>
         <v>122.78</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A76">
         <v>2026</v>
       </c>
       <c r="B76" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C76" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E76" t="s">
-        <v>26</v>
-      </c>
-      <c r="F76" s="2">
+        <v>8</v>
+      </c>
+      <c r="E76" s="2">
         <f t="shared" si="1"/>
         <v>2.9897727272727272</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A77">
         <v>2026</v>
       </c>
       <c r="B77" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C77" t="s">
+        <v>10</v>
+      </c>
+      <c r="D77" t="s">
         <v>11</v>
       </c>
-      <c r="D77" t="s">
-        <v>12</v>
-      </c>
-      <c r="E77" t="s">
-        <v>26</v>
-      </c>
-      <c r="F77" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="E77" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A78">
         <v>2026</v>
       </c>
       <c r="B78" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C78" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D78" t="s">
-        <v>12</v>
-      </c>
-      <c r="E78" t="s">
-        <v>26</v>
-      </c>
-      <c r="F78" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.5">
+        <v>11</v>
+      </c>
+      <c r="E78" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A79">
         <v>2026</v>
       </c>
       <c r="B79" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C79" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D79" t="s">
-        <v>12</v>
-      </c>
-      <c r="E79" t="s">
-        <v>26</v>
-      </c>
-      <c r="F79" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.5">
+        <v>11</v>
+      </c>
+      <c r="E79" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A80">
         <v>2026</v>
       </c>
       <c r="B80" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C80" t="s">
+        <v>14</v>
+      </c>
+      <c r="D80" t="s">
         <v>15</v>
       </c>
-      <c r="D80" t="s">
-        <v>16</v>
-      </c>
-      <c r="E80" t="s">
-        <v>26</v>
-      </c>
-      <c r="F80" s="2">
+      <c r="E80" s="2">
         <f t="shared" si="2"/>
         <v>2.6310000000000002</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A81">
         <v>2026</v>
       </c>
       <c r="B81" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C81" t="s">
+        <v>16</v>
+      </c>
+      <c r="D81" t="s">
         <v>17</v>
       </c>
-      <c r="D81" t="s">
-        <v>18</v>
-      </c>
-      <c r="E81" t="s">
-        <v>26</v>
-      </c>
-      <c r="F81" s="2">
+      <c r="E81" s="2">
         <f t="shared" si="3"/>
         <v>10.524000000000001</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A82">
         <v>2026</v>
       </c>
       <c r="B82" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C82" t="s">
+        <v>18</v>
+      </c>
+      <c r="D82" t="s">
         <v>19</v>
       </c>
-      <c r="D82" t="s">
-        <v>20</v>
-      </c>
-      <c r="E82" t="s">
-        <v>26</v>
-      </c>
-      <c r="F82" s="2">
+      <c r="E82" s="2">
         <f t="shared" si="4"/>
         <v>8.6464788732394382</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A83">
         <v>2026</v>
       </c>
       <c r="B83" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C83" t="s">
+        <v>20</v>
+      </c>
+      <c r="D83" t="s">
         <v>21</v>
       </c>
-      <c r="D83" t="s">
-        <v>22</v>
-      </c>
-      <c r="E83" t="s">
-        <v>26</v>
-      </c>
-      <c r="F83" s="2">
-        <f>F81*2</f>
+      <c r="E83" s="2">
+        <f>E81*2</f>
         <v>21.048000000000002</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A84">
         <v>2026</v>
       </c>
       <c r="B84" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C84" t="s">
+        <v>22</v>
+      </c>
+      <c r="D84" t="s">
         <v>23</v>
       </c>
-      <c r="D84" t="s">
-        <v>24</v>
-      </c>
-      <c r="E84" t="s">
-        <v>26</v>
-      </c>
-      <c r="F84" s="2">
-        <f>F76</f>
+      <c r="E84" s="2">
+        <f>E76</f>
         <v>2.9897727272727272</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A85">
         <v>2026</v>
       </c>
       <c r="B85" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C85" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D85" t="s">
-        <v>25</v>
-      </c>
-      <c r="E85" t="s">
-        <v>26</v>
-      </c>
-      <c r="F85" s="2">
+        <v>24</v>
+      </c>
+      <c r="E85" s="2">
         <v>0</v>
       </c>
     </row>
@@ -2277,8 +2015,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B4ECEDC51D0484091AFD4177D66ED73" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f94796c5baa2ef88ac6145701948dc8f">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b44fa922-a688-4301-8945-67f7597c9c55" xmlns:ns3="f6f44a7d-d6f5-4042-8792-19cb5f90fb06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e880ceb9264c792c54763cc60e020778" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B4ECEDC51D0484091AFD4177D66ED73" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cc653c178d9ffcb24786b6a9d53371f">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b44fa922-a688-4301-8945-67f7597c9c55" xmlns:ns3="f6f44a7d-d6f5-4042-8792-19cb5f90fb06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3af53c5407280ad7b07c166bc7f6511a" ns2:_="" ns3:_="">
     <xsd:import namespace="b44fa922-a688-4301-8945-67f7597c9c55"/>
     <xsd:import namespace="f6f44a7d-d6f5-4042-8792-19cb5f90fb06"/>
     <xsd:element name="properties">
@@ -2291,6 +2029,14 @@
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -2309,6 +2055,50 @@
     <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="12" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="13" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="14" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="18" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -2442,6 +2232,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2450,14 +2246,8 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F213A6A9-8AA2-4EFB-B08D-EEAF02FBEA26}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00375199-D6A3-486C-828F-7BFB0A9A5E72}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -2476,14 +2266,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{564AE492-6547-4D57-B909-D4ECF6985CEB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70733EE9-D017-4E55-9F72-DFA76D8EBF65}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="f6f44a7d-d6f5-4042-8792-19cb5f90fb06"/>
@@ -2498,4 +2280,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{564AE492-6547-4D57-B909-D4ECF6985CEB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>